<commit_message>
Actualizacion tablas al guardar
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaavi\Documents\laCartaDeNanaYRene\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isavo/Desktop/U/8º semestre/Construccion de Software/Repositorios/laCartaDeNanaYRene/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB4259B-6ED8-4F5C-9FED-56B122603884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D8BF87-6071-F345-AC80-5F118DC4EA7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5484" yWindow="3156" windowWidth="17280" windowHeight="8904" xr2:uid="{850194A8-4BCF-42A5-9864-108CD559B742}"/>
+    <workbookView xWindow="5480" yWindow="3160" windowWidth="17280" windowHeight="8900" xr2:uid="{850194A8-4BCF-42A5-9864-108CD559B742}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>queque</t>
   </si>
   <si>
-    <t>tartaleta</t>
-  </si>
-  <si>
     <t>pie de limon</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>crema, limon,merengue,harina, huevos</t>
+  </si>
+  <si>
+    <t>tartaleta durazno</t>
   </si>
 </sst>
 </file>
@@ -427,31 +427,31 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="36.5" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -459,13 +459,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>30000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -473,13 +473,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>700</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -487,35 +487,35 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>1000</v>

</xml_diff>